<commit_message>
SmokerStatus, policy level reserve interest
</commit_message>
<xml_diff>
--- a/examples/01_annuity_in_payment_simple/portfolio/portfolio_annuity_small.xlsx
+++ b/examples/01_annuity_in_payment_simple/portfolio/portfolio_annuity_small.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -50,25 +50,28 @@
   </si>
   <si>
     <t>AnnuityInPayment</t>
+  </si>
+  <si>
+    <t>RESERVING_RATE</t>
+  </si>
+  <si>
+    <t>SMOKERSTATUS</t>
+  </si>
+  <si>
+    <t>U</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFCE9178"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -91,10 +94,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -397,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -410,9 +412,13 @@
     <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -440,8 +446,14 @@
       <c r="I1" t="s">
         <v>10</v>
       </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>44561</v>
       </c>
@@ -463,16 +475,22 @@
       <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
         <v>11</v>
       </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11">
       <c r="A3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:11">
       <c r="A4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>

</xml_diff>

<commit_message>
B20 table added (still without select)
</commit_message>
<xml_diff>
--- a/examples/01_annuity_in_payment_simple/portfolio/portfolio_annuity_small.xlsx
+++ b/examples/01_annuity_in_payment_simple/portfolio/portfolio_annuity_small.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Oracle\PyProtolinc\examples\01_annuity_in_payment_simple\portfolio\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48644E72-8155-493E-AC6A-ED819790C861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="24915" windowHeight="12090"/>
+    <workbookView xWindow="-28920" yWindow="-420" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>ID</t>
   </si>
@@ -59,13 +65,16 @@
   </si>
   <si>
     <t>U</t>
+  </si>
+  <si>
+    <t>DATE_OF_DISABLEMENT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,7 +108,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -115,9 +124,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -155,9 +164,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -189,9 +198,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -223,9 +250,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -398,14 +443,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
@@ -418,7 +463,7 @@
     <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -452,8 +497,11 @@
       <c r="K1" t="s">
         <v>12</v>
       </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44561</v>
       </c>
@@ -484,13 +532,16 @@
       <c r="K2">
         <v>0</v>
       </c>
+      <c r="L2" s="1">
+        <v>44562</v>
+      </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>

</xml_diff>

<commit_message>
Started build of Cython Module
</commit_message>
<xml_diff>
--- a/examples/01_annuity_in_payment_simple/portfolio/portfolio_annuity_small.xlsx
+++ b/examples/01_annuity_in_payment_simple/portfolio/portfolio_annuity_small.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Oracle\PyProtolinc\examples\01_annuity_in_payment_simple\portfolio\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48644E72-8155-493E-AC6A-ED819790C861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-420" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-420" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -73,8 +67,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,7 +102,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -124,9 +118,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -164,9 +158,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -198,27 +192,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -250,27 +226,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -443,14 +401,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
@@ -463,7 +421,7 @@
     <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -501,7 +459,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>44561</v>
       </c>
@@ -536,12 +494,12 @@
         <v>44562</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>

</xml_diff>

<commit_message>
More fields in portfolio
</commit_message>
<xml_diff>
--- a/examples/01_annuity_in_payment_simple/portfolio/portfolio_annuity_small.xlsx
+++ b/examples/01_annuity_in_payment_simple/portfolio/portfolio_annuity_small.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming\py\PyProtolinc\examples\01_annuity_in_payment_simple\portfolio\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-420" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -37,9 +42,6 @@
     <t>SEX</t>
   </si>
   <si>
-    <t>m</t>
-  </si>
-  <si>
     <t>DIS1</t>
   </si>
   <si>
@@ -62,13 +64,16 @@
   </si>
   <si>
     <t>DATE_OF_DISABLEMENT</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,7 +107,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -118,9 +123,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -158,9 +163,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -192,9 +197,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -226,9 +232,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -401,14 +408,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
@@ -421,7 +428,7 @@
     <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -444,22 +451,22 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
       <c r="J1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44561</v>
       </c>
@@ -470,36 +477,36 @@
         <v>15454</v>
       </c>
       <c r="D2" s="1">
-        <v>44562</v>
+        <v>44530</v>
       </c>
       <c r="E2">
         <v>1200</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2" s="1">
-        <v>44562</v>
+        <v>44561</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>

</xml_diff>